<commit_message>
Simple Doughnut Chat Visualization in excel
</commit_message>
<xml_diff>
--- a/simple_Doughnut_chart_visualization.xlsx
+++ b/simple_Doughnut_chart_visualization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\ML_Project\Titanic_Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\ML_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Region</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Percentage revenue</t>
-  </si>
-  <si>
-    <t>helper</t>
   </si>
   <si>
     <t>NE</t>
@@ -59,7 +56,7 @@
     <t>MW</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Helper</t>
   </si>
 </sst>
 </file>
@@ -88,8 +85,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,9 +96,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -210,18 +207,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,7 +803,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$C$2:$D$2</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.19889468768857199</c:v>
@@ -1438,7 +1435,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$C$3:$D$3</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.22077874449183998</c:v>
@@ -2060,7 +2057,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$C$4:$D$4</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.17521269841255713</c:v>
@@ -2692,7 +2689,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$C$5:$D$5</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.17560027795268279</c:v>
@@ -3364,7 +3361,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$C$7:$D$7</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.11131951654971044</c:v>
@@ -3996,7 +3993,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$C$7:$D$7</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.11131951654971044</c:v>
@@ -8221,6 +8218,7 @@
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>NE</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="4000">
@@ -9056,8 +9054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -9065,6 +9063,7 @@
     <col min="1" max="1" width="8.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
@@ -9078,106 +9077,104 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>4</v>
+      <c r="A2" s="9" t="s">
+        <v>3</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="10">
         <v>311136664.049981</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="11">
         <v>0.19889468768857199</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="12">
         <f>1-[1]Sheet1!$C2</f>
         <v>0.80110531231142801</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>5</v>
+      <c r="A3" s="13" t="s">
+        <v>4</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="14">
         <v>345370521.71997762</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="15">
         <v>0.22077874449183998</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="16">
         <f>1-[1]Sheet1!$C3</f>
         <v>0.77922125550816002</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
+      <c r="A4" s="9" t="s">
+        <v>5</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="10">
         <v>274090249.04997832</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="11">
         <v>0.17521269841255713</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="12">
         <f>1-[1]Sheet1!$C4</f>
         <v>0.82478730158744284</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>7</v>
+      <c r="A5" s="13" t="s">
+        <v>6</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="14">
         <v>274696550.83998662</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="15">
         <v>0.17560027795268279</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="16">
         <f>1-[1]Sheet1!$C5</f>
         <v>0.82439972204731715</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
+      <c r="A6" s="9" t="s">
+        <v>7</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="10">
         <v>184894381.06000951</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="11">
         <v>0.11819407490463742</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="12">
         <f>1-[1]Sheet1!$C6</f>
         <v>0.8818059250953626</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="9" t="s">
-        <v>9</v>
+      <c r="A7" s="13" t="s">
+        <v>8</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="14">
         <v>174140312.27000734</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="15">
         <v>0.11131951654971044</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="16">
         <f>1-[1]Sheet1!$C7</f>
         <v>0.8886804834502896</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8">
         <f>SUBTOTAL(109,[1]Sheet1!$D$2:$D$7)</f>
         <v>5</v>
       </c>

</xml_diff>